<commit_message>
fix: ajuste e criação de mais uma rota
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,104 +436,302 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Qual o seu nome?</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Qual o seu email?</t>
+          <t>nome</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Você vem ao evento?</t>
+          <t>email</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Quais os nomes dos seus filhos?</t>
+          <t>evento</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Quais as idades dos seus filhos?</t>
+          <t>filhos</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>idades</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>pedro</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>teste@teste.com</t>
+          <t>dsadsada</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>sim</t>
+          <t>laerciogu01@gmail.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>testi, testando</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+          <t>dsa</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>dsadsadas</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>dasdsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dsadsadafgdg</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>laerciogu01@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>dsa</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>dsadsadas</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>dasdsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>fdsfdsfds</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>fsdfsfs</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>fsdfdsfs</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>fsfsdfds</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>fsdfds</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>tesnatdo</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>dsada</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>dasdasdas</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>dasdada</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>dasdsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>dsfdsfsdfsd</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>fsdfsdfs</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>fsdfsdfsfsd</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>fsdfsfsfds</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>fsdfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>fsdfsdfsd</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fdsfsfs</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>fsfdsfs</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>fsdfs</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>fsdfsfds</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>dsadasda</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>dasdsadasdsa</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>eeeeeeeeeeeeeee</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>eeeeeeeeeeeeeeee</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>eeeeeeeeeeeee</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>dsadsadas</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>dasdsa</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>dsada</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>dsadadada</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>fsdfsdfsd</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ssssssssssssss</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ssssssssssssssss</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ssssssssssssss</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>sssssssssssssss</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>thiago</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>teste</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>dsds</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>8</t>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>dsdsdsd</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>dsdsds</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>dsdsds</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>dsdsds</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>dsdsds</t>
         </is>
       </c>
     </row>

</xml_diff>